<commit_message>
Arreglo de error en rutas de documentos
</commit_message>
<xml_diff>
--- a/documentos/resultados.xlsx
+++ b/documentos/resultados.xlsx
@@ -452,11 +452,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2018-11-16 00:00:00</t>
+          <t>2018-11-01 00:00:00</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>2785</v>
       </c>
     </row>
     <row r="3">
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2018-11-17 00:00:00</t>
+          <t>2018-11-02 00:00:00</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -478,7 +478,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2018-11-18 00:00:00</t>
+          <t>2018-11-03 00:00:00</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -491,11 +491,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2018-11-19 00:00:00</t>
+          <t>2018-11-04 00:00:00</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>23</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6">
@@ -504,11 +504,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2018-11-20 00:00:00</t>
+          <t>2018-11-05 00:00:00</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>